<commit_message>
proberen save uit voorstellingController te gebruiken in ExcelController
</commit_message>
<xml_diff>
--- a/get_speeldata-bolwerk.xlsx
+++ b/get_speeldata-bolwerk.xlsx
@@ -256,7 +256,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-413]D/M/YYYY"/>
+    <numFmt numFmtId="165" formatCode="[$-413]DD/MM/YY\ HH:MM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -359,7 +359,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
@@ -414,7 +414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>16</v>
       </c>
@@ -452,7 +452,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>16</v>
       </c>
@@ -484,7 +484,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>16</v>
       </c>
@@ -516,7 +516,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>16</v>
       </c>
@@ -554,7 +554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -589,7 +589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>16</v>
       </c>
@@ -627,7 +627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>16</v>
       </c>
@@ -662,7 +662,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
@@ -700,7 +700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>16</v>
       </c>
@@ -738,7 +738,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>16</v>
       </c>
@@ -776,7 +776,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>16</v>
       </c>
@@ -805,7 +805,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>16</v>
       </c>
@@ -843,7 +843,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>16</v>
       </c>
@@ -881,7 +881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>16</v>
       </c>
@@ -913,7 +913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>16</v>
       </c>
@@ -951,7 +951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>16</v>
       </c>
@@ -989,7 +989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>16</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>16</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>16</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>16</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>16</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>16</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>16</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>16</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>16</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
jquery.js formule voor navbar aangepast, formule voor Excelbestand "document.ready" aan begin verwijderd, functioneerd nu weer. jqueryExcelUpload.js verwijderd
</commit_message>
<xml_diff>
--- a/get_speeldata-bolwerk.xlsx
+++ b/get_speeldata-bolwerk.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="77">
   <si>
     <t xml:space="preserve">Seizoen</t>
   </si>
@@ -248,15 +248,19 @@
   </si>
   <si>
     <t xml:space="preserve">Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul de Munnik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-413]DD/MM/YY\ HH:MM"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY\ HH:MM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -324,12 +328,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1360,6 +1368,44 @@
         <v>25</v>
       </c>
       <c r="P27" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>43974.875</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="O28" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="P28" s="0" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>